<commit_message>
checking rows and columns for layoutfiles again... still need to be not a complete overwrite, and addlayout needs to be implemented
</commit_message>
<xml_diff>
--- a/tests/testdata/project/layout.xlsx
+++ b/tests/testdata/project/layout.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="20">
   <si>
     <t># Layout for 2777.dbf</t>
   </si>
@@ -59,9 +59,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>empty</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
   </si>
   <si>
     <t>H</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -183,8 +177,8 @@
   </sheetPr>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -337,286 +331,286 @@
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -696,28 +690,28 @@
         <v>13</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,286 +719,286 @@
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>